<commit_message>
new changes but all working
</commit_message>
<xml_diff>
--- a/cafe94/src/main/java/data/Data.xlsx
+++ b/cafe94/src/main/java/data/Data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kiran\Desktop\Project\CAFE94\cafe94\src\main\java\data\"/>
     </mc:Choice>
@@ -23,7 +23,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="129">
   <si>
     <t>FirstName</t>
   </si>
@@ -477,11 +477,27 @@
   <si>
     <t>juhhh</t>
   </si>
+  <si>
+    <t xml:space="preserve">Basket CafeMate0007 has the following items:
+Item: Espresso, price: 1.00 pounds
+Item: Wrap, price: 1.00 pounds
+Item: DonkAsk, price: 1.00 pounds
+Item: Three, price: 1.00 pounds, quantity: 4
+Total cost: 7.00 pounds
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basket CafeMate0007 has the following items:
+Item: SoftDrink, price: 1.00 pounds
+Total cost: 1.00 pounds
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -852,221 +868,221 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.5546875" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="22.6640625" customWidth="1"/>
-    <col min="6" max="6" width="11.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.109375" customWidth="1"/>
-    <col min="8" max="8" width="11.77734375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="14.5546875"/>
+    <col min="2" max="2" customWidth="true" width="17.33203125"/>
+    <col min="3" max="3" customWidth="true" width="15.0"/>
+    <col min="4" max="4" customWidth="true" width="18.0"/>
+    <col min="5" max="5" customWidth="true" width="22.6640625"/>
+    <col min="6" max="6" customWidth="true" width="11.88671875"/>
+    <col min="7" max="7" customWidth="true" width="10.109375"/>
+    <col min="8" max="8" customWidth="true" width="11.77734375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>85</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s" s="0">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s" s="0">
         <v>87</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>89</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H3" t="s">
+      <c r="H3" t="s" s="0">
         <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>91</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>92</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>93</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>94</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" t="s" s="0">
         <v>68</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="s" s="0">
         <v>70</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" t="s" s="0">
         <v>71</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H5" t="s">
+      <c r="H5" t="s" s="0">
         <v>101</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>73</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>74</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>75</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>76</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>77</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" t="s" s="0">
         <v>79</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" t="s" s="0">
         <v>80</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" t="s" s="0">
         <v>81</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" t="s" s="0">
         <v>82</v>
       </c>
-      <c r="G7" t="s">
+      <c r="G7" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H7" t="s">
+      <c r="H7" t="s" s="0">
         <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>108</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>69</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>109</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" t="s" s="0">
         <v>110</v>
       </c>
-      <c r="G8" t="s">
+      <c r="G8" t="s" s="0">
         <v>111</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" t="s" s="0">
         <v>101</v>
       </c>
     </row>
@@ -1090,60 +1106,60 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.6640625"/>
+    <col min="3" max="3" customWidth="true" width="13.77734375"/>
+    <col min="6" max="6" customWidth="true" width="15.109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>119</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>120</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" t="s" s="0">
         <v>121</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" t="s" s="0">
         <v>4</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>124</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>126</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>125</v>
       </c>
     </row>
@@ -1165,116 +1181,131 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="18.44140625" customWidth="1"/>
-    <col min="4" max="4" width="18.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.77734375" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.88671875" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="17.77734375"/>
+    <col min="2" max="2" customWidth="true" width="18.33203125"/>
+    <col min="3" max="3" customWidth="true" width="18.44140625"/>
+    <col min="4" max="4" customWidth="true" width="18.88671875"/>
+    <col min="5" max="5" customWidth="true" width="17.33203125"/>
+    <col min="6" max="6" customWidth="true" width="15.77734375"/>
+    <col min="7" max="7" customWidth="true" width="14.44140625"/>
+    <col min="8" max="8" customWidth="true" width="12.88671875"/>
+    <col min="9" max="9" customWidth="true" width="13.33203125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B3">
+      <c r="B3" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B4">
+      <c r="B4" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>66</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6">
+      <c r="B6" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B7" s="0">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
         <v>107</v>
       </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" t="s">
-        <v>63</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="B8" t="s" s="0">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B9" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B10" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>33</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s" s="0">
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" t="s" s="0">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C12" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D12" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E12" t="n" s="0">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s" s="0">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>5</v>
+      <c r="B13" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="C13" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D13" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="E13" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>
@@ -1284,7 +1315,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2756A9DE-8640-4624-BF8F-A4CA2A44B7CF}">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1293,76 +1324,92 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>86</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>96</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>97</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>98</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>99</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>100</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>102</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" t="s" s="0">
         <v>106</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" t="s" s="0">
         <v>116</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" t="s" s="0">
         <v>117</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N2" t="s" s="0">
         <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>72</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" t="s" s="0">
         <v>112</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>107</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1381,16 +1428,16 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" t="s" s="0">
         <v>115</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" t="s" s="0">
         <v>114</v>
       </c>
     </row>
@@ -1409,340 +1456,340 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" customWidth="1"/>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.21875"/>
+    <col min="2" max="2" customWidth="true" width="16.5546875"/>
+    <col min="3" max="3" customWidth="true" width="17.21875"/>
+    <col min="4" max="4" customWidth="true" width="12.33203125"/>
+    <col min="5" max="5" customWidth="true" width="12.88671875"/>
+    <col min="6" max="6" customWidth="true" width="9.88671875"/>
+    <col min="7" max="7" customWidth="true" width="12.109375"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>64</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
+      <c r="B3" s="0">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0">
+        <v>1</v>
+      </c>
+      <c r="D3" s="0">
+        <v>1</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1</v>
+      </c>
+      <c r="F3" s="0">
+        <v>1</v>
+      </c>
+      <c r="G3" s="0">
+        <v>1</v>
+      </c>
+      <c r="H3" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>65</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>34</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>35</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>36</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>37</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" t="s" s="0">
         <v>38</v>
       </c>
-      <c r="H4" t="s">
+      <c r="H4" t="s" s="0">
         <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" t="s" s="0">
         <v>24</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
+      <c r="B5" s="0">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0">
+        <v>1</v>
+      </c>
+      <c r="D5" s="0">
+        <v>1</v>
+      </c>
+      <c r="E5" s="0">
+        <v>1</v>
+      </c>
+      <c r="F5" s="0">
+        <v>1</v>
+      </c>
+      <c r="G5" s="0">
+        <v>1</v>
+      </c>
+      <c r="H5" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" t="s" s="0">
         <v>41</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="0">
         <v>42</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" t="s" s="0">
         <v>43</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" t="s" s="0">
         <v>44</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="H6" t="s">
+      <c r="H6" t="s" s="0">
         <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" t="s" s="0">
         <v>25</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7">
-        <v>1</v>
-      </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>1</v>
-      </c>
-      <c r="H7">
+      <c r="B7" s="0">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" t="s" s="0">
         <v>47</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" t="s" s="0">
         <v>48</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" t="s" s="0">
         <v>50</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" t="s" s="0">
         <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="A9" t="s" s="0">
         <v>26</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9">
+      <c r="B9" s="0">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0">
+        <v>1</v>
+      </c>
+      <c r="D9" s="0">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" t="s" s="0">
         <v>62</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" t="s" s="0">
         <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" t="s" s="0">
         <v>27</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="0">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" t="s" s="0">
         <v>51</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" t="s" s="0">
         <v>52</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" t="s" s="0">
         <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" t="s" s="0">
         <v>28</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="0">
+        <v>1</v>
+      </c>
+      <c r="C13" s="0">
+        <v>1</v>
+      </c>
+      <c r="D13" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" t="s" s="0">
         <v>54</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" t="s" s="0">
         <v>57</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" t="s" s="0">
         <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="A15" t="s" s="0">
         <v>29</v>
       </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15">
-        <v>1</v>
-      </c>
-      <c r="D15">
+      <c r="B15" s="0">
+        <v>1</v>
+      </c>
+      <c r="C15" s="0">
+        <v>1</v>
+      </c>
+      <c r="D15" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" t="s" s="0">
         <v>55</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" t="s" s="0">
         <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="A17" t="s" s="0">
         <v>30</v>
       </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
+      <c r="B17" s="0">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="A18" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" t="s" s="0">
         <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+      <c r="A19" t="s" s="0">
         <v>31</v>
       </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19">
+      <c r="B19" s="0">
+        <v>1</v>
+      </c>
+      <c r="C19" s="0">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+      <c r="A20" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" t="s" s="0">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+      <c r="A21" t="s" s="0">
         <v>32</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="0">
         <v>1</v>
       </c>
     </row>
@@ -1762,15 +1809,15 @@
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>103</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>105</v>
       </c>
     </row>

</xml_diff>